<commit_message>
Added latest reports and more e2e tests
</commit_message>
<xml_diff>
--- a/API/reports/bug-report/Bug_Report.xlsx
+++ b/API/reports/bug-report/Bug_Report.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Fabio-Santoro\API\reports\bug-report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554BF0FB-0239-49F1-B32A-165FC801E062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FAE4F6-BB7C-46F0-A7E6-7B4A2A81C13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bug 1" sheetId="1" r:id="rId1"/>
     <sheet name="Bug 2" sheetId="3" r:id="rId2"/>
     <sheet name="Bug 3" sheetId="5" r:id="rId3"/>
     <sheet name="Bug 4" sheetId="6" r:id="rId4"/>
+    <sheet name="Bug 5" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="59">
   <si>
     <t>Category</t>
   </si>
@@ -123,9 +124,6 @@
     <t>Win 10</t>
   </si>
   <si>
-    <t>Version 93.0.4577.63</t>
-  </si>
-  <si>
     <t>Minor</t>
   </si>
   <si>
@@ -136,27 +134,6 @@
   </si>
   <si>
     <t>#3</t>
-  </si>
-  <si>
-    <t>http://automationpractice.multiformis.com</t>
-  </si>
-  <si>
-    <t>Search - No Validation on the frontend side is performed for any combination long combination of characters</t>
-  </si>
-  <si>
-    <t>The search box accepts long sequence of characters without performing any upfront validation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From the main page:
-1) Click on the search box and type any of the following a very long combination of characters
-2) Click on the magnifier icon (search Icon)
-</t>
-  </si>
-  <si>
-    <t>The form should perform upfront validation a long sequence to be accepted</t>
-  </si>
-  <si>
-    <t>I was able perform searches whith aforementioned long sequences. Although a meaningful message was displayed  (No results were found for your search), the unusual sequence was printed out on the screen  whioch could lead the browser  to crash or run out of memory</t>
   </si>
   <si>
     <t>#4</t>
@@ -196,12 +173,6 @@
     <t>The service returned a 200 Ok</t>
   </si>
   <si>
-    <t xml:space="preserve">Negative scenarios aimed at ensuring that validation was conducted at the backend for the following invalid scanrios did not accur : 
- 1) status(not in the enum range)
- 2) Invalid name (a digit/number)
-</t>
-  </si>
-  <si>
     <t>Missing required property in the Body is not validated while creating a new resource (POST /pet)</t>
   </si>
   <si>
@@ -233,16 +204,52 @@
     <t>Missing required property in the Body is not validated while updating a new resource (PUT /pet)</t>
   </si>
   <si>
-    <t xml:space="preserve">Negative scenarios aimed at ensuring that validation was conducted at the backend for the following invalid scanrios did not accur :
+    <t>MochaJs</t>
+  </si>
+  <si>
+    <t>Not easy to reproduce only happens for very fast chaned request</t>
+  </si>
+  <si>
+    <t>A 404 with an empty body is returned</t>
+  </si>
+  <si>
+    <t>Delay while creating a new Pet  (POST /pet) could result resource not found (404) to sesequent GET or DELETE requests</t>
+  </si>
+  <si>
+    <t>While creating a new pet I have noticed that intermittently there could be some delay between the returned response and the actual resource being created in the backend. This will result a failure of a subsequent calls to that resurce: either a GET /pet/{id} or DELETE /pet/{id} action in fact return a 404 with an empty body</t>
+  </si>
+  <si>
+    <t>Delay while creating a new Store order  (POST/store/order) could result resource not found (404) to sesequent GET or DELETE requests</t>
+  </si>
+  <si>
+    <t>While creating a new store order I have noticed that intermittently  there could be some delay between the returned response and the actual resource being created in the backend. This will result a failure of a subsequent calls to that resurce: either a GET /store/order/{id} or DELETE /store/order/{id} action in fact return a 404 with an empty body</t>
+  </si>
+  <si>
+    <t>The actual resource creation should be in synch with the response returned to the client (e.g. Postman or MochaJS etc.), for instance the response to the client should only be returned after checking that the resource is available from the source of information (e.g. DB etc)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative scenarios aimed at ensuring that, as per swagger, validation was conducted at the backend for the following invalid scenarios did not accur : 
+ 1) status(not in the enum range)
+ 2) Invalid name (a digit/number)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative scenarios aimed at ensuring that, as per swagger, validation was conducted at the backend for the following invalid scenarios did not accur :
 1) Missing required property "name"
 2) Missing required property "photoUrls"
  </t>
   </si>
   <si>
-    <t xml:space="preserve">Negative scenarios aimed at ensuring that validation was conducted at the backend for the following invalid scanrios did not accur :
+    <t xml:space="preserve">Negative scenarios aimed at ensuring that, as per swagger, validation was conducted at the backend for the following invalid scenarios did not accur :
 1) Missing required property "name"
 2) Missing required property "PhotoUrls"
  </t>
+  </si>
+  <si>
+    <t>Run the API automation suite multiple times. Eventually the problem will present</t>
+  </si>
+  <si>
+    <t>The actual resource creation should be in synch with the response returned to the client (e.g. Postman or MochaJS  etc.). For instance the response to the client should only be returned after checking that the resource is available from the source of information (e.g. DB etc)</t>
   </si>
 </sst>
 </file>
@@ -252,7 +259,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -286,12 +293,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="9"/>
@@ -375,11 +376,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -414,18 +414,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -547,7 +543,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>930544</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1476375</xdr:rowOff>
+      <xdr:rowOff>1076325</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -724,23 +720,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>592501</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>438150</xdr:rowOff>
+      <xdr:rowOff>235126</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>26851</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>760814</xdr:rowOff>
+      <xdr:colOff>770065</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>570857</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Immagine 2">
+        <xdr:cNvPr id="2" name="Immagine 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C81786A0-38AA-4629-A1A3-4B9A170C5ABE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21B46739-BFCD-4E5D-A2F4-63345388AFA2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -756,8 +752,57 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7298101" y="923925"/>
-          <a:ext cx="9054600" cy="6228164"/>
+          <a:off x="8029575" y="720901"/>
+          <a:ext cx="9066340" cy="3993331"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>617274</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>551798</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Immagine 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6376B330-211D-483C-B963-C0B498DA3D72}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7305675" y="1752600"/>
+          <a:ext cx="14809524" cy="5219048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1094,8 +1139,8 @@
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:E1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1135,7 +1180,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -1165,7 +1210,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -1174,8 +1219,8 @@
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>43</v>
+      <c r="C7" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="E7" s="11"/>
     </row>
@@ -1214,7 +1259,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="280.5" x14ac:dyDescent="0.2">
@@ -1225,7 +1270,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1234,7 +1279,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1243,13 +1288,13 @@
         <v>19</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="14"/>
     </row>
@@ -1261,7 +1306,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1279,7 +1324,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4267,7 +4312,7 @@
   <dimension ref="A1:E1002"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4298,7 +4343,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4307,7 +4352,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -4329,7 +4374,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>8</v>
       </c>
@@ -4337,7 +4382,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -4346,8 +4391,8 @@
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>43</v>
+      <c r="C7" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="E7" s="11"/>
     </row>
@@ -4386,7 +4431,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="242.25" x14ac:dyDescent="0.2">
@@ -4397,7 +4442,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4406,7 +4451,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4415,13 +4460,13 @@
         <v>19</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="14"/>
     </row>
@@ -4433,7 +4478,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -4451,7 +4496,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7432,8 +7477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841D423A-26D9-4268-BB8E-366BE6D9CB8E}">
   <dimension ref="A1:E1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7464,7 +7509,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -7473,7 +7518,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -7503,7 +7548,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -7512,8 +7557,8 @@
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>43</v>
+      <c r="C7" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="E7" s="11"/>
     </row>
@@ -7552,7 +7597,7 @@
         <v>15</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="242.25" x14ac:dyDescent="0.2">
@@ -7563,7 +7608,7 @@
         <v>17</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
@@ -7572,7 +7617,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
@@ -7581,13 +7626,13 @@
         <v>19</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="14"/>
     </row>
@@ -7599,7 +7644,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -7617,7 +7662,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10598,8 +10643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5852505-F041-4AA1-BD2E-4BDA22BC32A8}">
   <dimension ref="A1:E1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10630,7 +10675,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10639,7 +10684,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="E3" s="7"/>
     </row>
@@ -10661,7 +10706,7 @@
         <v>44454</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>8</v>
       </c>
@@ -10669,7 +10714,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="E6" s="9"/>
     </row>
@@ -10689,7 +10734,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10717,11 +10762,11 @@
       <c r="B11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="C11" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
         <v>16</v>
       </c>
@@ -10729,16 +10774,14 @@
         <v>17</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A13" s="18"/>
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="B13" s="5"/>
       <c r="C13" s="14" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -10747,13 +10790,13 @@
         <v>19</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="14"/>
     </row>
@@ -10765,7 +10808,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -10783,7 +10826,7 @@
         <v>24</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -13754,11 +13797,3172 @@
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A16:A18"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C7" r:id="rId1" xr:uid="{B364A250-57E5-40C1-AA5D-681C468EE14B}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CE9059-51B8-471C-B885-A725DEB2737E}">
+  <dimension ref="A1:E1002"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="57.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="19"/>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8">
+        <v>44454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="11"/>
+    </row>
+    <row r="8" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="19"/>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="19"/>
+      <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="19"/>
+      <c r="B15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C20" s="13"/>
+    </row>
+    <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C21" s="13"/>
+    </row>
+    <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C22" s="13"/>
+    </row>
+    <row r="23" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C23" s="13"/>
+    </row>
+    <row r="24" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C24" s="13"/>
+    </row>
+    <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C25" s="13"/>
+    </row>
+    <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C26" s="13"/>
+    </row>
+    <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C27" s="13"/>
+    </row>
+    <row r="28" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C28" s="13"/>
+    </row>
+    <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C29" s="13"/>
+    </row>
+    <row r="30" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C30" s="13"/>
+    </row>
+    <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C31" s="13"/>
+    </row>
+    <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C32" s="13"/>
+    </row>
+    <row r="33" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C33" s="13"/>
+    </row>
+    <row r="34" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C34" s="13"/>
+    </row>
+    <row r="35" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C35" s="13"/>
+    </row>
+    <row r="36" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C36" s="13"/>
+    </row>
+    <row r="37" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C37" s="13"/>
+    </row>
+    <row r="38" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C38" s="13"/>
+    </row>
+    <row r="39" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C39" s="13"/>
+    </row>
+    <row r="40" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C40" s="13"/>
+    </row>
+    <row r="41" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C41" s="13"/>
+    </row>
+    <row r="42" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C42" s="13"/>
+    </row>
+    <row r="43" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C43" s="13"/>
+    </row>
+    <row r="44" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C44" s="13"/>
+    </row>
+    <row r="45" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C45" s="13"/>
+    </row>
+    <row r="46" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C46" s="13"/>
+    </row>
+    <row r="47" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C47" s="13"/>
+    </row>
+    <row r="48" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C48" s="13"/>
+    </row>
+    <row r="49" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C49" s="13"/>
+    </row>
+    <row r="50" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C50" s="13"/>
+    </row>
+    <row r="51" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C51" s="13"/>
+    </row>
+    <row r="52" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C52" s="13"/>
+    </row>
+    <row r="53" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C53" s="13"/>
+    </row>
+    <row r="54" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C54" s="13"/>
+    </row>
+    <row r="55" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C55" s="13"/>
+    </row>
+    <row r="56" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C56" s="13"/>
+    </row>
+    <row r="57" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C57" s="13"/>
+    </row>
+    <row r="58" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C58" s="13"/>
+    </row>
+    <row r="59" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C59" s="13"/>
+    </row>
+    <row r="60" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C60" s="13"/>
+    </row>
+    <row r="61" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C61" s="13"/>
+    </row>
+    <row r="62" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C62" s="13"/>
+    </row>
+    <row r="63" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C63" s="13"/>
+    </row>
+    <row r="64" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C64" s="13"/>
+    </row>
+    <row r="65" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C65" s="13"/>
+    </row>
+    <row r="66" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C66" s="13"/>
+    </row>
+    <row r="67" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C67" s="13"/>
+    </row>
+    <row r="68" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C68" s="13"/>
+    </row>
+    <row r="69" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C69" s="13"/>
+    </row>
+    <row r="70" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C70" s="13"/>
+    </row>
+    <row r="71" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C71" s="13"/>
+    </row>
+    <row r="72" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C72" s="13"/>
+    </row>
+    <row r="73" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C73" s="13"/>
+    </row>
+    <row r="74" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C74" s="13"/>
+    </row>
+    <row r="75" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C75" s="13"/>
+    </row>
+    <row r="76" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C76" s="13"/>
+    </row>
+    <row r="77" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C77" s="13"/>
+    </row>
+    <row r="78" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C78" s="13"/>
+    </row>
+    <row r="79" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C79" s="13"/>
+    </row>
+    <row r="80" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C80" s="13"/>
+    </row>
+    <row r="81" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C81" s="13"/>
+    </row>
+    <row r="82" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C82" s="13"/>
+    </row>
+    <row r="83" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C83" s="13"/>
+    </row>
+    <row r="84" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C84" s="13"/>
+    </row>
+    <row r="85" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C85" s="13"/>
+    </row>
+    <row r="86" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C86" s="13"/>
+    </row>
+    <row r="87" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C87" s="13"/>
+    </row>
+    <row r="88" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C88" s="13"/>
+    </row>
+    <row r="89" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C89" s="13"/>
+    </row>
+    <row r="90" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C90" s="13"/>
+    </row>
+    <row r="91" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C91" s="13"/>
+    </row>
+    <row r="92" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C92" s="13"/>
+    </row>
+    <row r="93" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C93" s="13"/>
+    </row>
+    <row r="94" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C94" s="13"/>
+    </row>
+    <row r="95" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C95" s="13"/>
+    </row>
+    <row r="96" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C96" s="13"/>
+    </row>
+    <row r="97" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C97" s="13"/>
+    </row>
+    <row r="98" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C98" s="13"/>
+    </row>
+    <row r="99" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C99" s="13"/>
+    </row>
+    <row r="100" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C100" s="13"/>
+    </row>
+    <row r="101" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C101" s="13"/>
+    </row>
+    <row r="102" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C102" s="13"/>
+    </row>
+    <row r="103" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C103" s="13"/>
+    </row>
+    <row r="104" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C104" s="13"/>
+    </row>
+    <row r="105" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C105" s="13"/>
+    </row>
+    <row r="106" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C106" s="13"/>
+    </row>
+    <row r="107" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C107" s="13"/>
+    </row>
+    <row r="108" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C108" s="13"/>
+    </row>
+    <row r="109" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C109" s="13"/>
+    </row>
+    <row r="110" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C110" s="13"/>
+    </row>
+    <row r="111" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C111" s="13"/>
+    </row>
+    <row r="112" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C112" s="13"/>
+    </row>
+    <row r="113" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C113" s="13"/>
+    </row>
+    <row r="114" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C114" s="13"/>
+    </row>
+    <row r="115" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C115" s="13"/>
+    </row>
+    <row r="116" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C116" s="13"/>
+    </row>
+    <row r="117" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C117" s="13"/>
+    </row>
+    <row r="118" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C118" s="13"/>
+    </row>
+    <row r="119" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C119" s="13"/>
+    </row>
+    <row r="120" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C120" s="13"/>
+    </row>
+    <row r="121" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C121" s="13"/>
+    </row>
+    <row r="122" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C122" s="13"/>
+    </row>
+    <row r="123" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C123" s="13"/>
+    </row>
+    <row r="124" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C124" s="13"/>
+    </row>
+    <row r="125" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C125" s="13"/>
+    </row>
+    <row r="126" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C126" s="13"/>
+    </row>
+    <row r="127" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C127" s="13"/>
+    </row>
+    <row r="128" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C128" s="13"/>
+    </row>
+    <row r="129" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C129" s="13"/>
+    </row>
+    <row r="130" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C130" s="13"/>
+    </row>
+    <row r="131" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C131" s="13"/>
+    </row>
+    <row r="132" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C132" s="13"/>
+    </row>
+    <row r="133" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C133" s="13"/>
+    </row>
+    <row r="134" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C134" s="13"/>
+    </row>
+    <row r="135" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C135" s="13"/>
+    </row>
+    <row r="136" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C136" s="13"/>
+    </row>
+    <row r="137" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C137" s="13"/>
+    </row>
+    <row r="138" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C138" s="13"/>
+    </row>
+    <row r="139" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C139" s="13"/>
+    </row>
+    <row r="140" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C140" s="13"/>
+    </row>
+    <row r="141" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C141" s="13"/>
+    </row>
+    <row r="142" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C142" s="13"/>
+    </row>
+    <row r="143" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C143" s="13"/>
+    </row>
+    <row r="144" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C144" s="13"/>
+    </row>
+    <row r="145" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C145" s="13"/>
+    </row>
+    <row r="146" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C146" s="13"/>
+    </row>
+    <row r="147" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C147" s="13"/>
+    </row>
+    <row r="148" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C148" s="13"/>
+    </row>
+    <row r="149" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C149" s="13"/>
+    </row>
+    <row r="150" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C150" s="13"/>
+    </row>
+    <row r="151" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C151" s="13"/>
+    </row>
+    <row r="152" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C152" s="13"/>
+    </row>
+    <row r="153" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C153" s="13"/>
+    </row>
+    <row r="154" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C154" s="13"/>
+    </row>
+    <row r="155" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C155" s="13"/>
+    </row>
+    <row r="156" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C156" s="13"/>
+    </row>
+    <row r="157" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C157" s="13"/>
+    </row>
+    <row r="158" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C158" s="13"/>
+    </row>
+    <row r="159" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C159" s="13"/>
+    </row>
+    <row r="160" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C160" s="13"/>
+    </row>
+    <row r="161" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C161" s="13"/>
+    </row>
+    <row r="162" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C162" s="13"/>
+    </row>
+    <row r="163" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C163" s="13"/>
+    </row>
+    <row r="164" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C164" s="13"/>
+    </row>
+    <row r="165" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C165" s="13"/>
+    </row>
+    <row r="166" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C166" s="13"/>
+    </row>
+    <row r="167" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C167" s="13"/>
+    </row>
+    <row r="168" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C168" s="13"/>
+    </row>
+    <row r="169" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C169" s="13"/>
+    </row>
+    <row r="170" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C170" s="13"/>
+    </row>
+    <row r="171" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C171" s="13"/>
+    </row>
+    <row r="172" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C172" s="13"/>
+    </row>
+    <row r="173" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C173" s="13"/>
+    </row>
+    <row r="174" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C174" s="13"/>
+    </row>
+    <row r="175" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C175" s="13"/>
+    </row>
+    <row r="176" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C176" s="13"/>
+    </row>
+    <row r="177" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C177" s="13"/>
+    </row>
+    <row r="178" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C178" s="13"/>
+    </row>
+    <row r="179" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C179" s="13"/>
+    </row>
+    <row r="180" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C180" s="13"/>
+    </row>
+    <row r="181" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C181" s="13"/>
+    </row>
+    <row r="182" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C182" s="13"/>
+    </row>
+    <row r="183" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C183" s="13"/>
+    </row>
+    <row r="184" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C184" s="13"/>
+    </row>
+    <row r="185" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C185" s="13"/>
+    </row>
+    <row r="186" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C186" s="13"/>
+    </row>
+    <row r="187" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C187" s="13"/>
+    </row>
+    <row r="188" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C188" s="13"/>
+    </row>
+    <row r="189" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C189" s="13"/>
+    </row>
+    <row r="190" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C190" s="13"/>
+    </row>
+    <row r="191" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C191" s="13"/>
+    </row>
+    <row r="192" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C192" s="13"/>
+    </row>
+    <row r="193" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C193" s="13"/>
+    </row>
+    <row r="194" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C194" s="13"/>
+    </row>
+    <row r="195" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C195" s="13"/>
+    </row>
+    <row r="196" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C196" s="13"/>
+    </row>
+    <row r="197" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C197" s="13"/>
+    </row>
+    <row r="198" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C198" s="13"/>
+    </row>
+    <row r="199" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C199" s="13"/>
+    </row>
+    <row r="200" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C200" s="13"/>
+    </row>
+    <row r="201" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C201" s="13"/>
+    </row>
+    <row r="202" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C202" s="13"/>
+    </row>
+    <row r="203" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C203" s="13"/>
+    </row>
+    <row r="204" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C204" s="13"/>
+    </row>
+    <row r="205" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C205" s="13"/>
+    </row>
+    <row r="206" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C206" s="13"/>
+    </row>
+    <row r="207" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C207" s="13"/>
+    </row>
+    <row r="208" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C208" s="13"/>
+    </row>
+    <row r="209" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C209" s="13"/>
+    </row>
+    <row r="210" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C210" s="13"/>
+    </row>
+    <row r="211" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C211" s="13"/>
+    </row>
+    <row r="212" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C212" s="13"/>
+    </row>
+    <row r="213" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C213" s="13"/>
+    </row>
+    <row r="214" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C214" s="13"/>
+    </row>
+    <row r="215" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C215" s="13"/>
+    </row>
+    <row r="216" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C216" s="13"/>
+    </row>
+    <row r="217" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C217" s="13"/>
+    </row>
+    <row r="218" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C218" s="13"/>
+    </row>
+    <row r="219" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C219" s="13"/>
+    </row>
+    <row r="220" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C220" s="13"/>
+    </row>
+    <row r="221" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C221" s="13"/>
+    </row>
+    <row r="222" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C222" s="13"/>
+    </row>
+    <row r="223" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C223" s="13"/>
+    </row>
+    <row r="224" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C224" s="13"/>
+    </row>
+    <row r="225" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C225" s="13"/>
+    </row>
+    <row r="226" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C226" s="13"/>
+    </row>
+    <row r="227" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C227" s="13"/>
+    </row>
+    <row r="228" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C228" s="13"/>
+    </row>
+    <row r="229" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C229" s="13"/>
+    </row>
+    <row r="230" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C230" s="13"/>
+    </row>
+    <row r="231" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C231" s="13"/>
+    </row>
+    <row r="232" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C232" s="13"/>
+    </row>
+    <row r="233" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C233" s="13"/>
+    </row>
+    <row r="234" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C234" s="13"/>
+    </row>
+    <row r="235" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C235" s="13"/>
+    </row>
+    <row r="236" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C236" s="13"/>
+    </row>
+    <row r="237" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C237" s="13"/>
+    </row>
+    <row r="238" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C238" s="13"/>
+    </row>
+    <row r="239" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C239" s="13"/>
+    </row>
+    <row r="240" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C240" s="13"/>
+    </row>
+    <row r="241" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C241" s="13"/>
+    </row>
+    <row r="242" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C242" s="13"/>
+    </row>
+    <row r="243" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C243" s="13"/>
+    </row>
+    <row r="244" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C244" s="13"/>
+    </row>
+    <row r="245" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C245" s="13"/>
+    </row>
+    <row r="246" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C246" s="13"/>
+    </row>
+    <row r="247" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C247" s="13"/>
+    </row>
+    <row r="248" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C248" s="13"/>
+    </row>
+    <row r="249" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C249" s="13"/>
+    </row>
+    <row r="250" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C250" s="13"/>
+    </row>
+    <row r="251" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C251" s="13"/>
+    </row>
+    <row r="252" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C252" s="13"/>
+    </row>
+    <row r="253" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C253" s="13"/>
+    </row>
+    <row r="254" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C254" s="13"/>
+    </row>
+    <row r="255" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C255" s="13"/>
+    </row>
+    <row r="256" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C256" s="13"/>
+    </row>
+    <row r="257" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C257" s="13"/>
+    </row>
+    <row r="258" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C258" s="13"/>
+    </row>
+    <row r="259" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C259" s="13"/>
+    </row>
+    <row r="260" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C260" s="13"/>
+    </row>
+    <row r="261" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C261" s="13"/>
+    </row>
+    <row r="262" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C262" s="13"/>
+    </row>
+    <row r="263" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C263" s="13"/>
+    </row>
+    <row r="264" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C264" s="13"/>
+    </row>
+    <row r="265" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C265" s="13"/>
+    </row>
+    <row r="266" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C266" s="13"/>
+    </row>
+    <row r="267" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C267" s="13"/>
+    </row>
+    <row r="268" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C268" s="13"/>
+    </row>
+    <row r="269" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C269" s="13"/>
+    </row>
+    <row r="270" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C270" s="13"/>
+    </row>
+    <row r="271" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C271" s="13"/>
+    </row>
+    <row r="272" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C272" s="13"/>
+    </row>
+    <row r="273" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C273" s="13"/>
+    </row>
+    <row r="274" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C274" s="13"/>
+    </row>
+    <row r="275" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C275" s="13"/>
+    </row>
+    <row r="276" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C276" s="13"/>
+    </row>
+    <row r="277" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C277" s="13"/>
+    </row>
+    <row r="278" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C278" s="13"/>
+    </row>
+    <row r="279" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C279" s="13"/>
+    </row>
+    <row r="280" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C280" s="13"/>
+    </row>
+    <row r="281" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C281" s="13"/>
+    </row>
+    <row r="282" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C282" s="13"/>
+    </row>
+    <row r="283" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C283" s="13"/>
+    </row>
+    <row r="284" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C284" s="13"/>
+    </row>
+    <row r="285" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C285" s="13"/>
+    </row>
+    <row r="286" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C286" s="13"/>
+    </row>
+    <row r="287" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C287" s="13"/>
+    </row>
+    <row r="288" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C288" s="13"/>
+    </row>
+    <row r="289" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C289" s="13"/>
+    </row>
+    <row r="290" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C290" s="13"/>
+    </row>
+    <row r="291" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C291" s="13"/>
+    </row>
+    <row r="292" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C292" s="13"/>
+    </row>
+    <row r="293" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C293" s="13"/>
+    </row>
+    <row r="294" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C294" s="13"/>
+    </row>
+    <row r="295" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C295" s="13"/>
+    </row>
+    <row r="296" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C296" s="13"/>
+    </row>
+    <row r="297" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C297" s="13"/>
+    </row>
+    <row r="298" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C298" s="13"/>
+    </row>
+    <row r="299" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C299" s="13"/>
+    </row>
+    <row r="300" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C300" s="13"/>
+    </row>
+    <row r="301" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C301" s="13"/>
+    </row>
+    <row r="302" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C302" s="13"/>
+    </row>
+    <row r="303" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C303" s="13"/>
+    </row>
+    <row r="304" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C304" s="13"/>
+    </row>
+    <row r="305" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C305" s="13"/>
+    </row>
+    <row r="306" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C306" s="13"/>
+    </row>
+    <row r="307" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C307" s="13"/>
+    </row>
+    <row r="308" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C308" s="13"/>
+    </row>
+    <row r="309" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C309" s="13"/>
+    </row>
+    <row r="310" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C310" s="13"/>
+    </row>
+    <row r="311" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C311" s="13"/>
+    </row>
+    <row r="312" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C312" s="13"/>
+    </row>
+    <row r="313" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C313" s="13"/>
+    </row>
+    <row r="314" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C314" s="13"/>
+    </row>
+    <row r="315" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C315" s="13"/>
+    </row>
+    <row r="316" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C316" s="13"/>
+    </row>
+    <row r="317" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C317" s="13"/>
+    </row>
+    <row r="318" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C318" s="13"/>
+    </row>
+    <row r="319" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C319" s="13"/>
+    </row>
+    <row r="320" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C320" s="13"/>
+    </row>
+    <row r="321" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C321" s="13"/>
+    </row>
+    <row r="322" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C322" s="13"/>
+    </row>
+    <row r="323" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C323" s="13"/>
+    </row>
+    <row r="324" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C324" s="13"/>
+    </row>
+    <row r="325" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C325" s="13"/>
+    </row>
+    <row r="326" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C326" s="13"/>
+    </row>
+    <row r="327" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C327" s="13"/>
+    </row>
+    <row r="328" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C328" s="13"/>
+    </row>
+    <row r="329" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C329" s="13"/>
+    </row>
+    <row r="330" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C330" s="13"/>
+    </row>
+    <row r="331" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C331" s="13"/>
+    </row>
+    <row r="332" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C332" s="13"/>
+    </row>
+    <row r="333" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C333" s="13"/>
+    </row>
+    <row r="334" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C334" s="13"/>
+    </row>
+    <row r="335" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C335" s="13"/>
+    </row>
+    <row r="336" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C336" s="13"/>
+    </row>
+    <row r="337" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C337" s="13"/>
+    </row>
+    <row r="338" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C338" s="13"/>
+    </row>
+    <row r="339" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C339" s="13"/>
+    </row>
+    <row r="340" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C340" s="13"/>
+    </row>
+    <row r="341" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C341" s="13"/>
+    </row>
+    <row r="342" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C342" s="13"/>
+    </row>
+    <row r="343" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C343" s="13"/>
+    </row>
+    <row r="344" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C344" s="13"/>
+    </row>
+    <row r="345" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C345" s="13"/>
+    </row>
+    <row r="346" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C346" s="13"/>
+    </row>
+    <row r="347" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C347" s="13"/>
+    </row>
+    <row r="348" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C348" s="13"/>
+    </row>
+    <row r="349" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C349" s="13"/>
+    </row>
+    <row r="350" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C350" s="13"/>
+    </row>
+    <row r="351" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C351" s="13"/>
+    </row>
+    <row r="352" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C352" s="13"/>
+    </row>
+    <row r="353" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C353" s="13"/>
+    </row>
+    <row r="354" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C354" s="13"/>
+    </row>
+    <row r="355" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C355" s="13"/>
+    </row>
+    <row r="356" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C356" s="13"/>
+    </row>
+    <row r="357" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C357" s="13"/>
+    </row>
+    <row r="358" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C358" s="13"/>
+    </row>
+    <row r="359" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C359" s="13"/>
+    </row>
+    <row r="360" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C360" s="13"/>
+    </row>
+    <row r="361" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C361" s="13"/>
+    </row>
+    <row r="362" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C362" s="13"/>
+    </row>
+    <row r="363" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C363" s="13"/>
+    </row>
+    <row r="364" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C364" s="13"/>
+    </row>
+    <row r="365" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C365" s="13"/>
+    </row>
+    <row r="366" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C366" s="13"/>
+    </row>
+    <row r="367" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C367" s="13"/>
+    </row>
+    <row r="368" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C368" s="13"/>
+    </row>
+    <row r="369" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C369" s="13"/>
+    </row>
+    <row r="370" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C370" s="13"/>
+    </row>
+    <row r="371" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C371" s="13"/>
+    </row>
+    <row r="372" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C372" s="13"/>
+    </row>
+    <row r="373" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C373" s="13"/>
+    </row>
+    <row r="374" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C374" s="13"/>
+    </row>
+    <row r="375" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C375" s="13"/>
+    </row>
+    <row r="376" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C376" s="13"/>
+    </row>
+    <row r="377" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C377" s="13"/>
+    </row>
+    <row r="378" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C378" s="13"/>
+    </row>
+    <row r="379" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C379" s="13"/>
+    </row>
+    <row r="380" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C380" s="13"/>
+    </row>
+    <row r="381" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C381" s="13"/>
+    </row>
+    <row r="382" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C382" s="13"/>
+    </row>
+    <row r="383" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C383" s="13"/>
+    </row>
+    <row r="384" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C384" s="13"/>
+    </row>
+    <row r="385" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C385" s="13"/>
+    </row>
+    <row r="386" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C386" s="13"/>
+    </row>
+    <row r="387" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C387" s="13"/>
+    </row>
+    <row r="388" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C388" s="13"/>
+    </row>
+    <row r="389" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C389" s="13"/>
+    </row>
+    <row r="390" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C390" s="13"/>
+    </row>
+    <row r="391" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C391" s="13"/>
+    </row>
+    <row r="392" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C392" s="13"/>
+    </row>
+    <row r="393" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C393" s="13"/>
+    </row>
+    <row r="394" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C394" s="13"/>
+    </row>
+    <row r="395" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C395" s="13"/>
+    </row>
+    <row r="396" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C396" s="13"/>
+    </row>
+    <row r="397" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C397" s="13"/>
+    </row>
+    <row r="398" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C398" s="13"/>
+    </row>
+    <row r="399" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C399" s="13"/>
+    </row>
+    <row r="400" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C400" s="13"/>
+    </row>
+    <row r="401" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C401" s="13"/>
+    </row>
+    <row r="402" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C402" s="13"/>
+    </row>
+    <row r="403" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C403" s="13"/>
+    </row>
+    <row r="404" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C404" s="13"/>
+    </row>
+    <row r="405" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C405" s="13"/>
+    </row>
+    <row r="406" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C406" s="13"/>
+    </row>
+    <row r="407" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C407" s="13"/>
+    </row>
+    <row r="408" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C408" s="13"/>
+    </row>
+    <row r="409" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C409" s="13"/>
+    </row>
+    <row r="410" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C410" s="13"/>
+    </row>
+    <row r="411" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C411" s="13"/>
+    </row>
+    <row r="412" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C412" s="13"/>
+    </row>
+    <row r="413" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C413" s="13"/>
+    </row>
+    <row r="414" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C414" s="13"/>
+    </row>
+    <row r="415" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C415" s="13"/>
+    </row>
+    <row r="416" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C416" s="13"/>
+    </row>
+    <row r="417" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C417" s="13"/>
+    </row>
+    <row r="418" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C418" s="13"/>
+    </row>
+    <row r="419" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C419" s="13"/>
+    </row>
+    <row r="420" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C420" s="13"/>
+    </row>
+    <row r="421" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C421" s="13"/>
+    </row>
+    <row r="422" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C422" s="13"/>
+    </row>
+    <row r="423" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C423" s="13"/>
+    </row>
+    <row r="424" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C424" s="13"/>
+    </row>
+    <row r="425" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C425" s="13"/>
+    </row>
+    <row r="426" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C426" s="13"/>
+    </row>
+    <row r="427" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C427" s="13"/>
+    </row>
+    <row r="428" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C428" s="13"/>
+    </row>
+    <row r="429" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C429" s="13"/>
+    </row>
+    <row r="430" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C430" s="13"/>
+    </row>
+    <row r="431" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C431" s="13"/>
+    </row>
+    <row r="432" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C432" s="13"/>
+    </row>
+    <row r="433" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C433" s="13"/>
+    </row>
+    <row r="434" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C434" s="13"/>
+    </row>
+    <row r="435" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C435" s="13"/>
+    </row>
+    <row r="436" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C436" s="13"/>
+    </row>
+    <row r="437" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C437" s="13"/>
+    </row>
+    <row r="438" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C438" s="13"/>
+    </row>
+    <row r="439" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C439" s="13"/>
+    </row>
+    <row r="440" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C440" s="13"/>
+    </row>
+    <row r="441" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C441" s="13"/>
+    </row>
+    <row r="442" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C442" s="13"/>
+    </row>
+    <row r="443" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C443" s="13"/>
+    </row>
+    <row r="444" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C444" s="13"/>
+    </row>
+    <row r="445" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C445" s="13"/>
+    </row>
+    <row r="446" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C446" s="13"/>
+    </row>
+    <row r="447" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C447" s="13"/>
+    </row>
+    <row r="448" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C448" s="13"/>
+    </row>
+    <row r="449" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C449" s="13"/>
+    </row>
+    <row r="450" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C450" s="13"/>
+    </row>
+    <row r="451" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C451" s="13"/>
+    </row>
+    <row r="452" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C452" s="13"/>
+    </row>
+    <row r="453" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C453" s="13"/>
+    </row>
+    <row r="454" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C454" s="13"/>
+    </row>
+    <row r="455" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C455" s="13"/>
+    </row>
+    <row r="456" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C456" s="13"/>
+    </row>
+    <row r="457" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C457" s="13"/>
+    </row>
+    <row r="458" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C458" s="13"/>
+    </row>
+    <row r="459" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C459" s="13"/>
+    </row>
+    <row r="460" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C460" s="13"/>
+    </row>
+    <row r="461" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C461" s="13"/>
+    </row>
+    <row r="462" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C462" s="13"/>
+    </row>
+    <row r="463" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C463" s="13"/>
+    </row>
+    <row r="464" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C464" s="13"/>
+    </row>
+    <row r="465" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C465" s="13"/>
+    </row>
+    <row r="466" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C466" s="13"/>
+    </row>
+    <row r="467" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C467" s="13"/>
+    </row>
+    <row r="468" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C468" s="13"/>
+    </row>
+    <row r="469" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C469" s="13"/>
+    </row>
+    <row r="470" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C470" s="13"/>
+    </row>
+    <row r="471" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C471" s="13"/>
+    </row>
+    <row r="472" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C472" s="13"/>
+    </row>
+    <row r="473" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C473" s="13"/>
+    </row>
+    <row r="474" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C474" s="13"/>
+    </row>
+    <row r="475" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C475" s="13"/>
+    </row>
+    <row r="476" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C476" s="13"/>
+    </row>
+    <row r="477" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C477" s="13"/>
+    </row>
+    <row r="478" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C478" s="13"/>
+    </row>
+    <row r="479" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C479" s="13"/>
+    </row>
+    <row r="480" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C480" s="13"/>
+    </row>
+    <row r="481" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C481" s="13"/>
+    </row>
+    <row r="482" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C482" s="13"/>
+    </row>
+    <row r="483" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C483" s="13"/>
+    </row>
+    <row r="484" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C484" s="13"/>
+    </row>
+    <row r="485" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C485" s="13"/>
+    </row>
+    <row r="486" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C486" s="13"/>
+    </row>
+    <row r="487" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C487" s="13"/>
+    </row>
+    <row r="488" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C488" s="13"/>
+    </row>
+    <row r="489" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C489" s="13"/>
+    </row>
+    <row r="490" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C490" s="13"/>
+    </row>
+    <row r="491" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C491" s="13"/>
+    </row>
+    <row r="492" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C492" s="13"/>
+    </row>
+    <row r="493" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C493" s="13"/>
+    </row>
+    <row r="494" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C494" s="13"/>
+    </row>
+    <row r="495" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C495" s="13"/>
+    </row>
+    <row r="496" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C496" s="13"/>
+    </row>
+    <row r="497" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C497" s="13"/>
+    </row>
+    <row r="498" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C498" s="13"/>
+    </row>
+    <row r="499" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C499" s="13"/>
+    </row>
+    <row r="500" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C500" s="13"/>
+    </row>
+    <row r="501" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C501" s="13"/>
+    </row>
+    <row r="502" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C502" s="13"/>
+    </row>
+    <row r="503" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C503" s="13"/>
+    </row>
+    <row r="504" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C504" s="13"/>
+    </row>
+    <row r="505" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C505" s="13"/>
+    </row>
+    <row r="506" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C506" s="13"/>
+    </row>
+    <row r="507" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C507" s="13"/>
+    </row>
+    <row r="508" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C508" s="13"/>
+    </row>
+    <row r="509" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C509" s="13"/>
+    </row>
+    <row r="510" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C510" s="13"/>
+    </row>
+    <row r="511" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C511" s="13"/>
+    </row>
+    <row r="512" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C512" s="13"/>
+    </row>
+    <row r="513" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C513" s="13"/>
+    </row>
+    <row r="514" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C514" s="13"/>
+    </row>
+    <row r="515" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C515" s="13"/>
+    </row>
+    <row r="516" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C516" s="13"/>
+    </row>
+    <row r="517" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C517" s="13"/>
+    </row>
+    <row r="518" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C518" s="13"/>
+    </row>
+    <row r="519" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C519" s="13"/>
+    </row>
+    <row r="520" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C520" s="13"/>
+    </row>
+    <row r="521" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C521" s="13"/>
+    </row>
+    <row r="522" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C522" s="13"/>
+    </row>
+    <row r="523" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C523" s="13"/>
+    </row>
+    <row r="524" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C524" s="13"/>
+    </row>
+    <row r="525" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C525" s="13"/>
+    </row>
+    <row r="526" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C526" s="13"/>
+    </row>
+    <row r="527" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C527" s="13"/>
+    </row>
+    <row r="528" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C528" s="13"/>
+    </row>
+    <row r="529" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C529" s="13"/>
+    </row>
+    <row r="530" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C530" s="13"/>
+    </row>
+    <row r="531" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C531" s="13"/>
+    </row>
+    <row r="532" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C532" s="13"/>
+    </row>
+    <row r="533" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C533" s="13"/>
+    </row>
+    <row r="534" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C534" s="13"/>
+    </row>
+    <row r="535" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C535" s="13"/>
+    </row>
+    <row r="536" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C536" s="13"/>
+    </row>
+    <row r="537" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C537" s="13"/>
+    </row>
+    <row r="538" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C538" s="13"/>
+    </row>
+    <row r="539" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C539" s="13"/>
+    </row>
+    <row r="540" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C540" s="13"/>
+    </row>
+    <row r="541" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C541" s="13"/>
+    </row>
+    <row r="542" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C542" s="13"/>
+    </row>
+    <row r="543" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C543" s="13"/>
+    </row>
+    <row r="544" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C544" s="13"/>
+    </row>
+    <row r="545" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C545" s="13"/>
+    </row>
+    <row r="546" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C546" s="13"/>
+    </row>
+    <row r="547" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C547" s="13"/>
+    </row>
+    <row r="548" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C548" s="13"/>
+    </row>
+    <row r="549" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C549" s="13"/>
+    </row>
+    <row r="550" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C550" s="13"/>
+    </row>
+    <row r="551" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C551" s="13"/>
+    </row>
+    <row r="552" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C552" s="13"/>
+    </row>
+    <row r="553" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C553" s="13"/>
+    </row>
+    <row r="554" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C554" s="13"/>
+    </row>
+    <row r="555" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C555" s="13"/>
+    </row>
+    <row r="556" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C556" s="13"/>
+    </row>
+    <row r="557" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C557" s="13"/>
+    </row>
+    <row r="558" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C558" s="13"/>
+    </row>
+    <row r="559" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C559" s="13"/>
+    </row>
+    <row r="560" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C560" s="13"/>
+    </row>
+    <row r="561" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C561" s="13"/>
+    </row>
+    <row r="562" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C562" s="13"/>
+    </row>
+    <row r="563" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C563" s="13"/>
+    </row>
+    <row r="564" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C564" s="13"/>
+    </row>
+    <row r="565" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C565" s="13"/>
+    </row>
+    <row r="566" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C566" s="13"/>
+    </row>
+    <row r="567" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C567" s="13"/>
+    </row>
+    <row r="568" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C568" s="13"/>
+    </row>
+    <row r="569" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C569" s="13"/>
+    </row>
+    <row r="570" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C570" s="13"/>
+    </row>
+    <row r="571" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C571" s="13"/>
+    </row>
+    <row r="572" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C572" s="13"/>
+    </row>
+    <row r="573" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C573" s="13"/>
+    </row>
+    <row r="574" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C574" s="13"/>
+    </row>
+    <row r="575" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C575" s="13"/>
+    </row>
+    <row r="576" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C576" s="13"/>
+    </row>
+    <row r="577" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C577" s="13"/>
+    </row>
+    <row r="578" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C578" s="13"/>
+    </row>
+    <row r="579" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C579" s="13"/>
+    </row>
+    <row r="580" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C580" s="13"/>
+    </row>
+    <row r="581" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C581" s="13"/>
+    </row>
+    <row r="582" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C582" s="13"/>
+    </row>
+    <row r="583" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C583" s="13"/>
+    </row>
+    <row r="584" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C584" s="13"/>
+    </row>
+    <row r="585" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C585" s="13"/>
+    </row>
+    <row r="586" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C586" s="13"/>
+    </row>
+    <row r="587" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C587" s="13"/>
+    </row>
+    <row r="588" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C588" s="13"/>
+    </row>
+    <row r="589" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C589" s="13"/>
+    </row>
+    <row r="590" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C590" s="13"/>
+    </row>
+    <row r="591" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C591" s="13"/>
+    </row>
+    <row r="592" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C592" s="13"/>
+    </row>
+    <row r="593" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C593" s="13"/>
+    </row>
+    <row r="594" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C594" s="13"/>
+    </row>
+    <row r="595" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C595" s="13"/>
+    </row>
+    <row r="596" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C596" s="13"/>
+    </row>
+    <row r="597" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C597" s="13"/>
+    </row>
+    <row r="598" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C598" s="13"/>
+    </row>
+    <row r="599" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C599" s="13"/>
+    </row>
+    <row r="600" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C600" s="13"/>
+    </row>
+    <row r="601" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C601" s="13"/>
+    </row>
+    <row r="602" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C602" s="13"/>
+    </row>
+    <row r="603" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C603" s="13"/>
+    </row>
+    <row r="604" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C604" s="13"/>
+    </row>
+    <row r="605" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C605" s="13"/>
+    </row>
+    <row r="606" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C606" s="13"/>
+    </row>
+    <row r="607" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C607" s="13"/>
+    </row>
+    <row r="608" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C608" s="13"/>
+    </row>
+    <row r="609" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C609" s="13"/>
+    </row>
+    <row r="610" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C610" s="13"/>
+    </row>
+    <row r="611" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C611" s="13"/>
+    </row>
+    <row r="612" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C612" s="13"/>
+    </row>
+    <row r="613" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C613" s="13"/>
+    </row>
+    <row r="614" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C614" s="13"/>
+    </row>
+    <row r="615" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C615" s="13"/>
+    </row>
+    <row r="616" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C616" s="13"/>
+    </row>
+    <row r="617" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C617" s="13"/>
+    </row>
+    <row r="618" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C618" s="13"/>
+    </row>
+    <row r="619" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C619" s="13"/>
+    </row>
+    <row r="620" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C620" s="13"/>
+    </row>
+    <row r="621" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C621" s="13"/>
+    </row>
+    <row r="622" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C622" s="13"/>
+    </row>
+    <row r="623" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C623" s="13"/>
+    </row>
+    <row r="624" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C624" s="13"/>
+    </row>
+    <row r="625" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C625" s="13"/>
+    </row>
+    <row r="626" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C626" s="13"/>
+    </row>
+    <row r="627" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C627" s="13"/>
+    </row>
+    <row r="628" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C628" s="13"/>
+    </row>
+    <row r="629" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C629" s="13"/>
+    </row>
+    <row r="630" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C630" s="13"/>
+    </row>
+    <row r="631" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C631" s="13"/>
+    </row>
+    <row r="632" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C632" s="13"/>
+    </row>
+    <row r="633" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C633" s="13"/>
+    </row>
+    <row r="634" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C634" s="13"/>
+    </row>
+    <row r="635" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C635" s="13"/>
+    </row>
+    <row r="636" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C636" s="13"/>
+    </row>
+    <row r="637" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C637" s="13"/>
+    </row>
+    <row r="638" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C638" s="13"/>
+    </row>
+    <row r="639" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C639" s="13"/>
+    </row>
+    <row r="640" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C640" s="13"/>
+    </row>
+    <row r="641" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C641" s="13"/>
+    </row>
+    <row r="642" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C642" s="13"/>
+    </row>
+    <row r="643" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C643" s="13"/>
+    </row>
+    <row r="644" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C644" s="13"/>
+    </row>
+    <row r="645" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C645" s="13"/>
+    </row>
+    <row r="646" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C646" s="13"/>
+    </row>
+    <row r="647" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C647" s="13"/>
+    </row>
+    <row r="648" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C648" s="13"/>
+    </row>
+    <row r="649" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C649" s="13"/>
+    </row>
+    <row r="650" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C650" s="13"/>
+    </row>
+    <row r="651" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C651" s="13"/>
+    </row>
+    <row r="652" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C652" s="13"/>
+    </row>
+    <row r="653" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C653" s="13"/>
+    </row>
+    <row r="654" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C654" s="13"/>
+    </row>
+    <row r="655" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C655" s="13"/>
+    </row>
+    <row r="656" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C656" s="13"/>
+    </row>
+    <row r="657" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C657" s="13"/>
+    </row>
+    <row r="658" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C658" s="13"/>
+    </row>
+    <row r="659" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C659" s="13"/>
+    </row>
+    <row r="660" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C660" s="13"/>
+    </row>
+    <row r="661" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C661" s="13"/>
+    </row>
+    <row r="662" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C662" s="13"/>
+    </row>
+    <row r="663" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C663" s="13"/>
+    </row>
+    <row r="664" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C664" s="13"/>
+    </row>
+    <row r="665" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C665" s="13"/>
+    </row>
+    <row r="666" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C666" s="13"/>
+    </row>
+    <row r="667" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C667" s="13"/>
+    </row>
+    <row r="668" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C668" s="13"/>
+    </row>
+    <row r="669" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C669" s="13"/>
+    </row>
+    <row r="670" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C670" s="13"/>
+    </row>
+    <row r="671" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C671" s="13"/>
+    </row>
+    <row r="672" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C672" s="13"/>
+    </row>
+    <row r="673" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C673" s="13"/>
+    </row>
+    <row r="674" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C674" s="13"/>
+    </row>
+    <row r="675" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C675" s="13"/>
+    </row>
+    <row r="676" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C676" s="13"/>
+    </row>
+    <row r="677" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C677" s="13"/>
+    </row>
+    <row r="678" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C678" s="13"/>
+    </row>
+    <row r="679" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C679" s="13"/>
+    </row>
+    <row r="680" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C680" s="13"/>
+    </row>
+    <row r="681" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C681" s="13"/>
+    </row>
+    <row r="682" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C682" s="13"/>
+    </row>
+    <row r="683" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C683" s="13"/>
+    </row>
+    <row r="684" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C684" s="13"/>
+    </row>
+    <row r="685" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C685" s="13"/>
+    </row>
+    <row r="686" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C686" s="13"/>
+    </row>
+    <row r="687" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C687" s="13"/>
+    </row>
+    <row r="688" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C688" s="13"/>
+    </row>
+    <row r="689" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C689" s="13"/>
+    </row>
+    <row r="690" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C690" s="13"/>
+    </row>
+    <row r="691" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C691" s="13"/>
+    </row>
+    <row r="692" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C692" s="13"/>
+    </row>
+    <row r="693" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C693" s="13"/>
+    </row>
+    <row r="694" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C694" s="13"/>
+    </row>
+    <row r="695" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C695" s="13"/>
+    </row>
+    <row r="696" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C696" s="13"/>
+    </row>
+    <row r="697" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C697" s="13"/>
+    </row>
+    <row r="698" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C698" s="13"/>
+    </row>
+    <row r="699" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C699" s="13"/>
+    </row>
+    <row r="700" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C700" s="13"/>
+    </row>
+    <row r="701" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C701" s="13"/>
+    </row>
+    <row r="702" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C702" s="13"/>
+    </row>
+    <row r="703" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C703" s="13"/>
+    </row>
+    <row r="704" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C704" s="13"/>
+    </row>
+    <row r="705" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C705" s="13"/>
+    </row>
+    <row r="706" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C706" s="13"/>
+    </row>
+    <row r="707" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C707" s="13"/>
+    </row>
+    <row r="708" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C708" s="13"/>
+    </row>
+    <row r="709" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C709" s="13"/>
+    </row>
+    <row r="710" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C710" s="13"/>
+    </row>
+    <row r="711" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C711" s="13"/>
+    </row>
+    <row r="712" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C712" s="13"/>
+    </row>
+    <row r="713" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C713" s="13"/>
+    </row>
+    <row r="714" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C714" s="13"/>
+    </row>
+    <row r="715" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C715" s="13"/>
+    </row>
+    <row r="716" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C716" s="13"/>
+    </row>
+    <row r="717" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C717" s="13"/>
+    </row>
+    <row r="718" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C718" s="13"/>
+    </row>
+    <row r="719" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C719" s="13"/>
+    </row>
+    <row r="720" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C720" s="13"/>
+    </row>
+    <row r="721" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C721" s="13"/>
+    </row>
+    <row r="722" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C722" s="13"/>
+    </row>
+    <row r="723" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C723" s="13"/>
+    </row>
+    <row r="724" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C724" s="13"/>
+    </row>
+    <row r="725" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C725" s="13"/>
+    </row>
+    <row r="726" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C726" s="13"/>
+    </row>
+    <row r="727" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C727" s="13"/>
+    </row>
+    <row r="728" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C728" s="13"/>
+    </row>
+    <row r="729" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C729" s="13"/>
+    </row>
+    <row r="730" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C730" s="13"/>
+    </row>
+    <row r="731" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C731" s="13"/>
+    </row>
+    <row r="732" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C732" s="13"/>
+    </row>
+    <row r="733" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C733" s="13"/>
+    </row>
+    <row r="734" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C734" s="13"/>
+    </row>
+    <row r="735" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C735" s="13"/>
+    </row>
+    <row r="736" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C736" s="13"/>
+    </row>
+    <row r="737" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C737" s="13"/>
+    </row>
+    <row r="738" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C738" s="13"/>
+    </row>
+    <row r="739" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C739" s="13"/>
+    </row>
+    <row r="740" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C740" s="13"/>
+    </row>
+    <row r="741" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C741" s="13"/>
+    </row>
+    <row r="742" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C742" s="13"/>
+    </row>
+    <row r="743" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C743" s="13"/>
+    </row>
+    <row r="744" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C744" s="13"/>
+    </row>
+    <row r="745" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C745" s="13"/>
+    </row>
+    <row r="746" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C746" s="13"/>
+    </row>
+    <row r="747" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C747" s="13"/>
+    </row>
+    <row r="748" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C748" s="13"/>
+    </row>
+    <row r="749" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C749" s="13"/>
+    </row>
+    <row r="750" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C750" s="13"/>
+    </row>
+    <row r="751" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C751" s="13"/>
+    </row>
+    <row r="752" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C752" s="13"/>
+    </row>
+    <row r="753" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C753" s="13"/>
+    </row>
+    <row r="754" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C754" s="13"/>
+    </row>
+    <row r="755" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C755" s="13"/>
+    </row>
+    <row r="756" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C756" s="13"/>
+    </row>
+    <row r="757" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C757" s="13"/>
+    </row>
+    <row r="758" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C758" s="13"/>
+    </row>
+    <row r="759" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C759" s="13"/>
+    </row>
+    <row r="760" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C760" s="13"/>
+    </row>
+    <row r="761" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C761" s="13"/>
+    </row>
+    <row r="762" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C762" s="13"/>
+    </row>
+    <row r="763" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C763" s="13"/>
+    </row>
+    <row r="764" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C764" s="13"/>
+    </row>
+    <row r="765" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C765" s="13"/>
+    </row>
+    <row r="766" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C766" s="13"/>
+    </row>
+    <row r="767" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C767" s="13"/>
+    </row>
+    <row r="768" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C768" s="13"/>
+    </row>
+    <row r="769" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C769" s="13"/>
+    </row>
+    <row r="770" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C770" s="13"/>
+    </row>
+    <row r="771" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C771" s="13"/>
+    </row>
+    <row r="772" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C772" s="13"/>
+    </row>
+    <row r="773" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C773" s="13"/>
+    </row>
+    <row r="774" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C774" s="13"/>
+    </row>
+    <row r="775" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C775" s="13"/>
+    </row>
+    <row r="776" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C776" s="13"/>
+    </row>
+    <row r="777" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C777" s="13"/>
+    </row>
+    <row r="778" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C778" s="13"/>
+    </row>
+    <row r="779" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C779" s="13"/>
+    </row>
+    <row r="780" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C780" s="13"/>
+    </row>
+    <row r="781" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C781" s="13"/>
+    </row>
+    <row r="782" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C782" s="13"/>
+    </row>
+    <row r="783" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C783" s="13"/>
+    </row>
+    <row r="784" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C784" s="13"/>
+    </row>
+    <row r="785" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C785" s="13"/>
+    </row>
+    <row r="786" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C786" s="13"/>
+    </row>
+    <row r="787" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C787" s="13"/>
+    </row>
+    <row r="788" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C788" s="13"/>
+    </row>
+    <row r="789" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C789" s="13"/>
+    </row>
+    <row r="790" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C790" s="13"/>
+    </row>
+    <row r="791" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C791" s="13"/>
+    </row>
+    <row r="792" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C792" s="13"/>
+    </row>
+    <row r="793" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C793" s="13"/>
+    </row>
+    <row r="794" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C794" s="13"/>
+    </row>
+    <row r="795" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C795" s="13"/>
+    </row>
+    <row r="796" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C796" s="13"/>
+    </row>
+    <row r="797" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C797" s="13"/>
+    </row>
+    <row r="798" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C798" s="13"/>
+    </row>
+    <row r="799" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C799" s="13"/>
+    </row>
+    <row r="800" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C800" s="13"/>
+    </row>
+    <row r="801" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C801" s="13"/>
+    </row>
+    <row r="802" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C802" s="13"/>
+    </row>
+    <row r="803" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C803" s="13"/>
+    </row>
+    <row r="804" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C804" s="13"/>
+    </row>
+    <row r="805" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C805" s="13"/>
+    </row>
+    <row r="806" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C806" s="13"/>
+    </row>
+    <row r="807" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C807" s="13"/>
+    </row>
+    <row r="808" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C808" s="13"/>
+    </row>
+    <row r="809" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C809" s="13"/>
+    </row>
+    <row r="810" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C810" s="13"/>
+    </row>
+    <row r="811" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C811" s="13"/>
+    </row>
+    <row r="812" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C812" s="13"/>
+    </row>
+    <row r="813" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C813" s="13"/>
+    </row>
+    <row r="814" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C814" s="13"/>
+    </row>
+    <row r="815" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C815" s="13"/>
+    </row>
+    <row r="816" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C816" s="13"/>
+    </row>
+    <row r="817" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C817" s="13"/>
+    </row>
+    <row r="818" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C818" s="13"/>
+    </row>
+    <row r="819" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C819" s="13"/>
+    </row>
+    <row r="820" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C820" s="13"/>
+    </row>
+    <row r="821" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C821" s="13"/>
+    </row>
+    <row r="822" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C822" s="13"/>
+    </row>
+    <row r="823" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C823" s="13"/>
+    </row>
+    <row r="824" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C824" s="13"/>
+    </row>
+    <row r="825" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C825" s="13"/>
+    </row>
+    <row r="826" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C826" s="13"/>
+    </row>
+    <row r="827" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C827" s="13"/>
+    </row>
+    <row r="828" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C828" s="13"/>
+    </row>
+    <row r="829" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C829" s="13"/>
+    </row>
+    <row r="830" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C830" s="13"/>
+    </row>
+    <row r="831" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C831" s="13"/>
+    </row>
+    <row r="832" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C832" s="13"/>
+    </row>
+    <row r="833" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C833" s="13"/>
+    </row>
+    <row r="834" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C834" s="13"/>
+    </row>
+    <row r="835" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C835" s="13"/>
+    </row>
+    <row r="836" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C836" s="13"/>
+    </row>
+    <row r="837" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C837" s="13"/>
+    </row>
+    <row r="838" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C838" s="13"/>
+    </row>
+    <row r="839" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C839" s="13"/>
+    </row>
+    <row r="840" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C840" s="13"/>
+    </row>
+    <row r="841" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C841" s="13"/>
+    </row>
+    <row r="842" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C842" s="13"/>
+    </row>
+    <row r="843" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C843" s="13"/>
+    </row>
+    <row r="844" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C844" s="13"/>
+    </row>
+    <row r="845" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C845" s="13"/>
+    </row>
+    <row r="846" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C846" s="13"/>
+    </row>
+    <row r="847" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C847" s="13"/>
+    </row>
+    <row r="848" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C848" s="13"/>
+    </row>
+    <row r="849" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C849" s="13"/>
+    </row>
+    <row r="850" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C850" s="13"/>
+    </row>
+    <row r="851" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C851" s="13"/>
+    </row>
+    <row r="852" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C852" s="13"/>
+    </row>
+    <row r="853" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C853" s="13"/>
+    </row>
+    <row r="854" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C854" s="13"/>
+    </row>
+    <row r="855" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C855" s="13"/>
+    </row>
+    <row r="856" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C856" s="13"/>
+    </row>
+    <row r="857" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C857" s="13"/>
+    </row>
+    <row r="858" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C858" s="13"/>
+    </row>
+    <row r="859" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C859" s="13"/>
+    </row>
+    <row r="860" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C860" s="13"/>
+    </row>
+    <row r="861" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C861" s="13"/>
+    </row>
+    <row r="862" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C862" s="13"/>
+    </row>
+    <row r="863" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C863" s="13"/>
+    </row>
+    <row r="864" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C864" s="13"/>
+    </row>
+    <row r="865" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C865" s="13"/>
+    </row>
+    <row r="866" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C866" s="13"/>
+    </row>
+    <row r="867" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C867" s="13"/>
+    </row>
+    <row r="868" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C868" s="13"/>
+    </row>
+    <row r="869" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C869" s="13"/>
+    </row>
+    <row r="870" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C870" s="13"/>
+    </row>
+    <row r="871" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C871" s="13"/>
+    </row>
+    <row r="872" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C872" s="13"/>
+    </row>
+    <row r="873" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C873" s="13"/>
+    </row>
+    <row r="874" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C874" s="13"/>
+    </row>
+    <row r="875" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C875" s="13"/>
+    </row>
+    <row r="876" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C876" s="13"/>
+    </row>
+    <row r="877" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C877" s="13"/>
+    </row>
+    <row r="878" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C878" s="13"/>
+    </row>
+    <row r="879" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C879" s="13"/>
+    </row>
+    <row r="880" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C880" s="13"/>
+    </row>
+    <row r="881" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C881" s="13"/>
+    </row>
+    <row r="882" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C882" s="13"/>
+    </row>
+    <row r="883" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C883" s="13"/>
+    </row>
+    <row r="884" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C884" s="13"/>
+    </row>
+    <row r="885" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C885" s="13"/>
+    </row>
+    <row r="886" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C886" s="13"/>
+    </row>
+    <row r="887" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C887" s="13"/>
+    </row>
+    <row r="888" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C888" s="13"/>
+    </row>
+    <row r="889" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C889" s="13"/>
+    </row>
+    <row r="890" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C890" s="13"/>
+    </row>
+    <row r="891" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C891" s="13"/>
+    </row>
+    <row r="892" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C892" s="13"/>
+    </row>
+    <row r="893" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C893" s="13"/>
+    </row>
+    <row r="894" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C894" s="13"/>
+    </row>
+    <row r="895" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C895" s="13"/>
+    </row>
+    <row r="896" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C896" s="13"/>
+    </row>
+    <row r="897" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C897" s="13"/>
+    </row>
+    <row r="898" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C898" s="13"/>
+    </row>
+    <row r="899" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C899" s="13"/>
+    </row>
+    <row r="900" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C900" s="13"/>
+    </row>
+    <row r="901" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C901" s="13"/>
+    </row>
+    <row r="902" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C902" s="13"/>
+    </row>
+    <row r="903" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C903" s="13"/>
+    </row>
+    <row r="904" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C904" s="13"/>
+    </row>
+    <row r="905" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C905" s="13"/>
+    </row>
+    <row r="906" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C906" s="13"/>
+    </row>
+    <row r="907" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C907" s="13"/>
+    </row>
+    <row r="908" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C908" s="13"/>
+    </row>
+    <row r="909" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C909" s="13"/>
+    </row>
+    <row r="910" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C910" s="13"/>
+    </row>
+    <row r="911" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C911" s="13"/>
+    </row>
+    <row r="912" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C912" s="13"/>
+    </row>
+    <row r="913" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C913" s="13"/>
+    </row>
+    <row r="914" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C914" s="13"/>
+    </row>
+    <row r="915" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C915" s="13"/>
+    </row>
+    <row r="916" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C916" s="13"/>
+    </row>
+    <row r="917" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C917" s="13"/>
+    </row>
+    <row r="918" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C918" s="13"/>
+    </row>
+    <row r="919" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C919" s="13"/>
+    </row>
+    <row r="920" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C920" s="13"/>
+    </row>
+    <row r="921" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C921" s="13"/>
+    </row>
+    <row r="922" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C922" s="13"/>
+    </row>
+    <row r="923" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C923" s="13"/>
+    </row>
+    <row r="924" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C924" s="13"/>
+    </row>
+    <row r="925" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C925" s="13"/>
+    </row>
+    <row r="926" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C926" s="13"/>
+    </row>
+    <row r="927" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C927" s="13"/>
+    </row>
+    <row r="928" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C928" s="13"/>
+    </row>
+    <row r="929" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C929" s="13"/>
+    </row>
+    <row r="930" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C930" s="13"/>
+    </row>
+    <row r="931" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C931" s="13"/>
+    </row>
+    <row r="932" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C932" s="13"/>
+    </row>
+    <row r="933" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C933" s="13"/>
+    </row>
+    <row r="934" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C934" s="13"/>
+    </row>
+    <row r="935" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C935" s="13"/>
+    </row>
+    <row r="936" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C936" s="13"/>
+    </row>
+    <row r="937" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C937" s="13"/>
+    </row>
+    <row r="938" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C938" s="13"/>
+    </row>
+    <row r="939" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C939" s="13"/>
+    </row>
+    <row r="940" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C940" s="13"/>
+    </row>
+    <row r="941" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C941" s="13"/>
+    </row>
+    <row r="942" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C942" s="13"/>
+    </row>
+    <row r="943" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C943" s="13"/>
+    </row>
+    <row r="944" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C944" s="13"/>
+    </row>
+    <row r="945" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C945" s="13"/>
+    </row>
+    <row r="946" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C946" s="13"/>
+    </row>
+    <row r="947" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C947" s="13"/>
+    </row>
+    <row r="948" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C948" s="13"/>
+    </row>
+    <row r="949" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C949" s="13"/>
+    </row>
+    <row r="950" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C950" s="13"/>
+    </row>
+    <row r="951" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C951" s="13"/>
+    </row>
+    <row r="952" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C952" s="13"/>
+    </row>
+    <row r="953" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C953" s="13"/>
+    </row>
+    <row r="954" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C954" s="13"/>
+    </row>
+    <row r="955" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C955" s="13"/>
+    </row>
+    <row r="956" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C956" s="13"/>
+    </row>
+    <row r="957" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C957" s="13"/>
+    </row>
+    <row r="958" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C958" s="13"/>
+    </row>
+    <row r="959" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C959" s="13"/>
+    </row>
+    <row r="960" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C960" s="13"/>
+    </row>
+    <row r="961" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C961" s="13"/>
+    </row>
+    <row r="962" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C962" s="13"/>
+    </row>
+    <row r="963" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C963" s="13"/>
+    </row>
+    <row r="964" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C964" s="13"/>
+    </row>
+    <row r="965" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C965" s="13"/>
+    </row>
+    <row r="966" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C966" s="13"/>
+    </row>
+    <row r="967" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C967" s="13"/>
+    </row>
+    <row r="968" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C968" s="13"/>
+    </row>
+    <row r="969" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C969" s="13"/>
+    </row>
+    <row r="970" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C970" s="13"/>
+    </row>
+    <row r="971" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C971" s="13"/>
+    </row>
+    <row r="972" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C972" s="13"/>
+    </row>
+    <row r="973" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C973" s="13"/>
+    </row>
+    <row r="974" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C974" s="13"/>
+    </row>
+    <row r="975" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C975" s="13"/>
+    </row>
+    <row r="976" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C976" s="13"/>
+    </row>
+    <row r="977" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C977" s="13"/>
+    </row>
+    <row r="978" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C978" s="13"/>
+    </row>
+    <row r="979" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C979" s="13"/>
+    </row>
+    <row r="980" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C980" s="13"/>
+    </row>
+    <row r="981" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C981" s="13"/>
+    </row>
+    <row r="982" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C982" s="13"/>
+    </row>
+    <row r="983" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C983" s="13"/>
+    </row>
+    <row r="984" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C984" s="13"/>
+    </row>
+    <row r="985" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C985" s="13"/>
+    </row>
+    <row r="986" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C986" s="13"/>
+    </row>
+    <row r="987" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C987" s="13"/>
+    </row>
+    <row r="988" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C988" s="13"/>
+    </row>
+    <row r="989" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C989" s="13"/>
+    </row>
+    <row r="990" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C990" s="13"/>
+    </row>
+    <row r="991" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C991" s="13"/>
+    </row>
+    <row r="992" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C992" s="13"/>
+    </row>
+    <row r="993" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C993" s="13"/>
+    </row>
+    <row r="994" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C994" s="13"/>
+    </row>
+    <row r="995" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C995" s="13"/>
+    </row>
+    <row r="996" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C996" s="13"/>
+    </row>
+    <row r="997" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C997" s="13"/>
+    </row>
+    <row r="998" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C998" s="13"/>
+    </row>
+    <row r="999" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C999" s="13"/>
+    </row>
+    <row r="1000" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C1000" s="13"/>
+    </row>
+    <row r="1001" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C1001" s="13"/>
+    </row>
+    <row r="1002" spans="3:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C1002" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A18"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>